<commit_message>
Atualizando cores dos times, como sugerido no PR #5
</commit_message>
<xml_diff>
--- a/data-raw/xlsx/teams.xlsx
+++ b/data-raw/xlsx/teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wamorim/Documents/williamorim/brasileirao/data-raw/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Mioto_OneDrive\Bruno\R-packages\brasileirao\data-raw\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFF0860-CFFA-1447-9426-D46CA756993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6767460B-270B-4031-8676-D58339355D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="162">
   <si>
     <t>Athletico PR</t>
   </si>
@@ -320,6 +320,192 @@
   </si>
   <si>
     <t>team</t>
+  </si>
+  <si>
+    <t>color1</t>
+  </si>
+  <si>
+    <t>color2</t>
+  </si>
+  <si>
+    <t>#007242</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
+  </si>
+  <si>
+    <t>#ff1100</t>
+  </si>
+  <si>
+    <t>#e43031</t>
+  </si>
+  <si>
+    <t>#231f20</t>
+  </si>
+  <si>
+    <t>#dc1212</t>
+  </si>
+  <si>
+    <t>#010101</t>
+  </si>
+  <si>
+    <t>#1f1a17</t>
+  </si>
+  <si>
+    <t>#0b5b8d</t>
+  </si>
+  <si>
+    <t>#2762a6</t>
+  </si>
+  <si>
+    <t>#cd3529</t>
+  </si>
+  <si>
+    <t>#f5e145</t>
+  </si>
+  <si>
+    <t>#cf192e</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#0f2d5b</t>
+  </si>
+  <si>
+    <t>#e41349</t>
+  </si>
+  <si>
+    <t>#f6dc01</t>
+  </si>
+  <si>
+    <t>#009b45</t>
+  </si>
+  <si>
+    <t>#fefefe</t>
+  </si>
+  <si>
+    <t>#026b38</t>
+  </si>
+  <si>
+    <t>#1e1214</t>
+  </si>
+  <si>
+    <t>#d82531</t>
+  </si>
+  <si>
+    <t>#006755</t>
+  </si>
+  <si>
+    <t>#f4cf16</t>
+  </si>
+  <si>
+    <t>#1f150a</t>
+  </si>
+  <si>
+    <t>#1e3d8e</t>
+  </si>
+  <si>
+    <t>#041e5c</t>
+  </si>
+  <si>
+    <t>#016c32</t>
+  </si>
+  <si>
+    <t>#ffdb01</t>
+  </si>
+  <si>
+    <t>#03a550</t>
+  </si>
+  <si>
+    <t>#c3281e</t>
+  </si>
+  <si>
+    <t>#070308</t>
+  </si>
+  <si>
+    <t>#870a28</t>
+  </si>
+  <si>
+    <t>#00613c</t>
+  </si>
+  <si>
+    <t>#1f5ea1</t>
+  </si>
+  <si>
+    <t>#e1251b</t>
+  </si>
+  <si>
+    <t>#26603c</t>
+  </si>
+  <si>
+    <t>#0e93d2</t>
+  </si>
+  <si>
+    <t>#006e4d</t>
+  </si>
+  <si>
+    <t>#e5050f</t>
+  </si>
+  <si>
+    <t>#64b054</t>
+  </si>
+  <si>
+    <t>#cc262d</t>
+  </si>
+  <si>
+    <t>#ee3338</t>
+  </si>
+  <si>
+    <t>#118e4c</t>
+  </si>
+  <si>
+    <t>#ed2129</t>
+  </si>
+  <si>
+    <t>#006437</t>
+  </si>
+  <si>
+    <t>#304296</t>
+  </si>
+  <si>
+    <t>#263484</t>
+  </si>
+  <si>
+    <t>#fbfbfb</t>
+  </si>
+  <si>
+    <t>#fdfdfd</t>
+  </si>
+  <si>
+    <t>#198538</t>
+  </si>
+  <si>
+    <t>#ee2722</t>
+  </si>
+  <si>
+    <t>#ee3124</t>
+  </si>
+  <si>
+    <t>#267946</t>
+  </si>
+  <si>
+    <t>#2d3492</t>
+  </si>
+  <si>
+    <t>#034ea2</t>
+  </si>
+  <si>
+    <t>#00a651</t>
+  </si>
+  <si>
+    <t>#ed1c24</t>
+  </si>
+  <si>
+    <t>#d91a21</t>
+  </si>
+  <si>
+    <t>#ffda00</t>
   </si>
 </sst>
 </file>
@@ -363,10 +549,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,20 +861,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -695,8 +884,14 @@
       <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -706,8 +901,14 @@
       <c r="C2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -717,8 +918,14 @@
       <c r="C3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -728,8 +935,14 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -739,8 +952,14 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -750,8 +969,14 @@
       <c r="C6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -761,8 +986,14 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -772,8 +1003,14 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -783,8 +1020,14 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -794,8 +1037,14 @@
       <c r="C10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -805,8 +1054,14 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -816,8 +1071,14 @@
       <c r="C12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -827,8 +1088,14 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -838,8 +1105,14 @@
       <c r="C14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -849,8 +1122,14 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -860,8 +1139,14 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -871,8 +1156,14 @@
       <c r="C17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -882,8 +1173,14 @@
       <c r="C18" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -893,8 +1190,14 @@
       <c r="C19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -904,8 +1207,14 @@
       <c r="C20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -915,8 +1224,14 @@
       <c r="C21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -926,8 +1241,14 @@
       <c r="C22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -937,8 +1258,14 @@
       <c r="C23" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -948,8 +1275,14 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -959,8 +1292,14 @@
       <c r="C25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -970,8 +1309,14 @@
       <c r="C26" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -981,8 +1326,14 @@
       <c r="C27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -992,8 +1343,14 @@
       <c r="C28" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1003,8 +1360,14 @@
       <c r="C29" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1014,8 +1377,14 @@
       <c r="C30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1025,8 +1394,14 @@
       <c r="C31" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1036,8 +1411,14 @@
       <c r="C32" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1047,8 +1428,14 @@
       <c r="C33" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1058,8 +1445,14 @@
       <c r="C34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1069,8 +1462,14 @@
       <c r="C35" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1080,8 +1479,14 @@
       <c r="C36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1091,8 +1496,14 @@
       <c r="C37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1102,8 +1513,14 @@
       <c r="C38" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1113,8 +1530,14 @@
       <c r="C39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1124,8 +1547,14 @@
       <c r="C40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -1135,8 +1564,14 @@
       <c r="C41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -1146,8 +1581,14 @@
       <c r="C42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1157,8 +1598,14 @@
       <c r="C43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -1168,8 +1615,14 @@
       <c r="C44" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -1178,6 +1631,12 @@
       </c>
       <c r="C45" t="s">
         <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>